<commit_message>
minor modification to add new cell to existing spreadsheet and save it as a new sheet
</commit_message>
<xml_diff>
--- a/xlsreader/output.xlsx
+++ b/xlsreader/output.xlsx
@@ -18,16 +18,94 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>CHANDAN TRADERS,CHANDAN TRADERS,C.K.C  BRIKS  FIELD,C.K.C  BRIKS  FIELD,C.K.C  BRIKS  FIELD,CEMENT TRADERS,CHAND BRICKS FIELD,CHAND BRICKS FIELD,CHAND BRICKS FIELD,CHAND BRICKS FIELD,CHANDAN TRADERS,CHATURTH BHRATA STORES,CHAUDHARY VASTRALYA,CHAUHAN ENT UDYOG,CHAUHAN ENT UDYOG,CHAUHAN ENT UDYOG,CHAUHAN ENT UDYOG,CHAUHAN ENT UDYOG,CHAUHAN ENT UDYOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAURASIA BROTHERS,CHAURASIA BROTHERS,CHIRAG AGENCIES,CHIRAG AGENCIES,CHIRAG AGENCIES,CHIRAG AGENCIES,CHIRAG AGENCIES,CHOTE LAL DHIRAJ KUMAR SARRAF,CHOTE LAL DHIRAJ KUMAR SARRAF,CIELO SEWING MACHINE COMPANY,COOL BREEZE SERVICES,COOL BREEZE SERVICES</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>HANUMANT BRICKS FIELD,HANUMANT BRICKS FIELD,HIMANSU TRADERS,HIMANSU TRADERS,HANUMANT ASSOCIATE,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI OM TRADERS,HARI OM TRADERS,HARI OM TRADERS,HARIOM AUTOMOBILE,HARIOM AUTOMOBILE,HARISH CHANDRA JAISWAL,HARISH CHANDRA JAISWAL,HARISH CHANDRA JAISWAL,HARISH CHANDRA JAISWAL,HARSE  ENTERPRISES,HARSH  ENTERPRISES,HARSH  ENTERPRISES,HARSH ENTERPRISES,HARSHITA COAL ENTERPRISES,HEMANT BRICKS FIELD,HEMANT BRICKS FIELD,HEMANT BRICKS FIELD,HEMANT BRICKS FIELD,HEMANT BRICKS FIELD,HEMANT BRICKS FIELD,HIMALYA TRADERS,HIND CONSTRUCTIONS,HIND CONSTRUCTIONS,HINDUSTAN ALMIRAH,HOSIERY HOUSE,HINDUSTAN TRADERS,HINDUSTAN TRADERS,HINDUSTAN TRADERS,HINDUSTAN TRADERS,HINDUSTAN TRADERS</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>J. A. S.  BRICKS FILED,JAI MAA AMBEY TRADERS,JAI MAA AMBEY TRADERS,JAI MAA AMBEY TRADERS,JAI MAA VAISHNO TRADERS,JAI MATA DI KHAD BHANDAR,JAISWAL AUTO MOBILES,JAISWAL AUTO MOBILES,JAISWAL TRADERS,J.K.TRADERS,J.K.TRADERS,J.P. ENTERPRISES,J.P. ENTERPRISES,J.P. ENTERPRISES,J.P. ENTERPRISES,JAG GANGA SETH  JEWELLERS,JAGDAMBIKA FILLING STAION,JAGDISH  PRASAD,JAGMAG FIREWORKS,JAI AMBEY TRADING CO.,JAI AMBEY TRADING CO.,JAI AMBEY TRADING CO.,JAI MAA DURGE,JAI MAA KALI HARVESTERS,JAI MAA VAISHNO DEVI TRADERS,JAI MAA VASHNO TRADERS,JAI MAA VASHNO TRADERS,JAI MAA VASHNO TRADERS,JAI MAA VASHNO TRADERS,JAI PRAKASH SARAF AND COMPANY,JAI PRAKASH SARAF AND COMPANY,JAI SRI RAM HOSIERY,JAIPRAKASH CHAURASIA,JAISWAL BRICKS FIELD,JAISWAL BRICKS FIELD,JAISWAL BRICKS FIELD,JAISWAL BUILDING MATERIAL,JAISWAL BUILDING MATERIAL,JAISWAL MACHINARY,JAISWAL MACHINARY,JAISWAL MEDICAL STORES,JAISWAL MEDICAL STORES,JAISWAL TRADERS,JAISWAL TRADERS,JAISWAL TRADERS,JAISWAL TRADERS,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING COMPANY,JANATA HARDWARE CENTER,JANTA BUILDING MATERIALS,JANTA CIMENT STORES,JANTA TRADERS,JANTA TRADERS,JANTA TRADING CO.,JANTA TRADING CO.,JAWAHAR MEDICAL STORES,JAY CYCELS,JAYSWAL TRADERS,J.K.GARMENTS</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>K D ENTERPRISES,KASAUDHAN JEWELLERS,KISHORI LAL SURENDRA KUMAR SARRAF,K G N TRADERS,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K.C.Y.  MARKA INT BHATTHA,K.C.Y.  MARKA INT BHATTHA,K.S.K.,K.S.K.,K.S.K.,KAILASH HOSIERY,KAILASH HOSIERY,KAMAZ VECTRA MOTORS LTD.,KAMAZ VECTRA MOTORS LTD.,KAMAZ VECTRA MOTORS LTD.,KANAK JEWELLERS,KANAK JEWELLERS,KANCHAN MOBILE WORLD,KANCHAN MOBILE WORLD,KANCHAN MOBILE WORLD,KANHA JEWELLERS,KANHA JEWELLERS,KANHAIYA GENERAL STORE,KAPIL DEV BRICKS FIELD,KAPIL DEV BRICKS FIELD,KASAUDHAN TRADERS,KATWARU SARAF AND CO.,KEDIA HOSIERY,KESHAV HOSIERY,KESHAV HOSIERY,KESHAV HOSIERY,KISAN EINT BHATTA,KISAN EINT BHATTA,KISAN EINT BHATTA,KISAN KHAD BHANDAR,KISAN SEWA KENDRA,KISAN SEWA KENDRA,KISAN SEWA KENDRA,KISAN SEWA KENDRA,KISHAN URVARAK KENDRA,KISHAN URVARAK KENDRA,KRISH ENTERPRISES,KRISHAK SEWA KENDRA,KRISHANKANT  INDANE GRAMIN VITARAK,KRISHANKANT  INDANE GRAMIN VITARAK,KRISHI SEWA KENDRA,KRISHI SEWA KENDRA,KRISHNA BIHARI LAL JWELLERS PVT.LTD.,KRISHNA BIHARI LAL JWELLERS PVT.LTD.,KRISHNA BRICKS FIELD,KRISHNA BRICKS FIELD,KRISHNA BRICKS FIELD,KRISHNA BRICKS FIELD,KRISHNA PACKAGING SOLUTION,KRISHNA PACKAGING SOLUTION,KRISHNA READYMADE CENTER,KRISHNA READYMADE CENTER,KUMAR AGENCIES,KUMAR AGENCIES,KUMAR TRADING CO,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,K.K. BRICKS FIELD,K.K. BRICKS FIELD,K.K. BRICKS FIELD,Krishna Feling Station,Krishna Feling Station</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>S S ENTERPRISES,S. K. TRADERS,SACHIN MINERAL WATER,SADBHAWANA ENTERPRISES,SADBHAWANA ENTERPRISES,SAI TREDERS,SAMINFRATECH INDIA,SANTOSHI TRADERS,SHANU ELECTRONICS,SHIV ENTERPRISES,SHREE AUTOMOBILES,SHRI DURGA ENTERPRISES,SHRI VAIBHAW STATIONERY AND ELECTRIC,SINGH BUILDING MATERIALS,SWARGIYA SHRI KANSHIRAM FOUNDATION,S K ENTERPRISES,S. ENTERPRISES,S.D. CHAURASIYA KIRANA STORE,S.D. CHAURASIYA KIRANA STORE,S.D. CHAURASIYA KIRANA STORE,S.K. ELECTRICALS,S.K. ENTERPRISES,S.K.JWELLERS,S.P. BRICKS FIELD,S.P. BRICKS FIELD,S.P. BRICKS FIELD,S.P. BRICKS FIELD,S.P. BRICKS FIELD,S.P. BRICKS FIELD,S.P. ENTERPRISES,S.P. ENTERPRISES,S.P. ENTERPRISES,S.S.CAITRERS,SADHU BRICKS FIELD,SAHANI CYCLE STORES,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAKSHI ENTERPRISES,SAM SPORTS,SANDEEP ENTERPRISES,SANDEEP HARDWARE &amp; PAINTS,SANGAM ENTERPRISES,SANGAM RICE MILL,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY CHAND,SANJAY KUMAR GUPTA,SANJAY KUMAR GUPTA,SANTOSH COAL DIPO,SAR ENTERPRISES,SARASVATI TRADERS,SARASVATI TRADERS,SARASVATI TRADERS,SARASVATI TRADERS,SARASVATI TRADERS,SARASVATI TRADERS,SAROJ COMMUNICATION,SAROJ COMMUNICATION,SAROJ COMMUNICATION,SATNAM MACHINES,SATNAM MACHINES,SATNAM MACHINES,SATNAM MACHINES,SATNAM MACHINES,SATNAM MACHINES,SATNAM MACHINES,SATYA ENTERPRISES,SHAHEED J.K.TRIPATHI AUTOMOBILES,SHAHEED J.K.TRIPATHI AUTOMOBILES,SHAHID J.K.TRIPATHI AUTO MOBILES,SHAIVVI TRADERS,SHAKTI INT UDHOGH,SHAKTI INT UDHOGH,SHAKUNTALA   JWELLERS,SHAKUNTALA   JWELLERS,SHANKAR AUTO  MOBILES,SHANKAR AUTO  MOBILES,SHANKAR AUTO  MOBILES,SHANKAR AUTO  MOBILES,SHARDA TRADERS,SHARDA TRADERS,SHARDA TRADERS,SHAREEF DUPATTA PALACE,SHEKHAR TRADERS,SHIBLEE  TRADERS,SHIBLEE  TRADERS,SHIBLEE ENTERPRISES,SHIV AUTO SALES,SHIV SHAKTI BRICKS FIELD,SHIV SHAKTI ENTERPRISES,SHIV SHAKTI ENTERPRISES,SHIV SHAKTI GALLA BHANDAR,SHIV SHAKTI MADERN RICE MILL,SHIV SHAKTI MADERN RICE MILL,SHIV SHAKTI TRADERS,SHIV SHAKTI TRADERS,SHIV SHAKTI TRADERS,SHIV SHAKTI TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIVA AGENCIES,SHIVA AGENCIES,SHIVA ENGINEERING STORE,SHIVA ENGINEERING STORE,SHIVA TRADERS,SHIVA TRADERS,SHIVA TRADERS,SHIVA TRADERS,SHIVA TRADERS,SHIVA TRADERS,SHIVAM ASSOCIATES,SHIVAM ASSOCIATES,SHIVAM ASSOCIATES,SHIVAM ENTERPRISES,SHIVAM ENTERPRISES,SHIVAM KIRANA STORE,SHIVAM TRADERS,SHIVAM TRADERS,SHIVESH JEWELLERS,SHRADHA ELECTRICAL &amp; ELECTRONICS,SHREE  SHYAM JWELLERS,SHREE BALAJI GARMENTS,SHREE BRICKS FIELD,SHREE JOYTI JEWELLERS,SHREE LAXMI GARMENTS,SHREE LAXMI GARMENTS,SHREE MAA SHEETALA JEWELLERS,SHREE MAHABIR  TRADING  COMPANY,SHREE MAHAKAL ASSOCIATES,SHREE PURSHOTTAM JEWELLERY HOUSE,SHREE SHREE  SAI NATH SWEET HOUSE,SHREE SHREE  SAI NATH SWEET HOUSE,SHREE SHREE  SAI NATH SWEET HOUSE,SHREE SHREE  SAI NATH SWEET HOUSE,SHRI DURGA GARMENTS,SHRI DURGA GARMENTS,SHRI HARI GARMENTS,SHRI JYOTI DHARMKANTA AND JEWLLERS,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI LAXMI TRADING CO.,SHRI LAXMI TRADING CO.,SHRI LUXMI TRADERS,SHRI LUXMI TRADERS,SHRI LUXMI TRADERS,SHRI NAV DURGA TRADING COMPANY,SHRI VIGHNESHWAR STEELS AND HARDWARE CENTER,SHYAM ENTERPRISES,SHYAM SUNDAR MANISH KUMAR SARRAF,SHYAMENDRA SHAHI,SINGH AUTOMOBILES,SINGH AUTOMOBILES,SINGH AUTOMOBILES,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH ENT BHATTHA,SINGH ENT BHATTHA,SINGH ENT BHATTHA,SINGH MEDICAL STORE,SINGH MEDICAL STORE,SINGH TRADERS,SINGH TRADERS,SINGH TRADERS,SINGH TRADERS,SITA RAM GANESH PRASAD SARAF,SITA RAM GANESH PRASAD SARAF,SONBARSA BRICKS FIELD,SONBARSA BRICKS FIELD,SONBARSA BRICKS FIELD,SREE RAPTI TRADERS,SRI  BALAJI JEWELLERS,SRI AMBEY  JEWELLERS,SRI AMBEY  JEWELLERS,SRI BALAJI AUTO SALES,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI SAI TRADING COMPANY,SRI SATYAM GARMENTS,SRI SATYAM GARMENTS,SRI SHANKER ENTERPRISES,STAR BAG HOUSE,STAR HANDLOOM AND HOSIERY SALE,STAR HANDLOOM AND HOSIERY SALE,STAR REFRIGERATION,SUBHAM DISTRIBUTORS,SUBHAM DISTRIBUTORS,SUBHAS BUILDING MATERIALS,SUBHASH MEDICAL STORES,SUDAMA BHARAT GAS GRAMIN VITRAK,SUDAMA BHARAT GAS GRAMIN VITRAK,SUNIL JWELLERS,SUNNY ELECTRONICS,SUNNY ELECTRONICS,SUNNY ELECTRONICS,SUNNY ELECTRONICS,SUNNY ELECTRONICS,SUPER STONE CRUSHER,SUPER STONE CRUSHER,SURAJ BEEJ BHANDAR,SURAJ ENTERPRISES,SURYANSH CONSTRUCTION &amp; SUPPLIERS,SUSHIL ENTERPRISES,SUSHIL ENTERPRISES,SUSHIL ENTERPRISES,SUSHIL ENTERPRISES,SUSHIL KUMAR MANISH KUMAR SARRAF,SUSHIL KUMAR MANISH KUMAR SARRAF,SWYANGAR ASSOCIATES,SWYANGAR ASSOCIATES,SWYANGAR ASSOCIATES,S.P.TRADERS,SANJAI PLASTIC TRADERS,SANJAI PLASTIC TRADERS</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>YASH ENTERPRISES,YASH GARMENT,YADAV AGENCY,YADAV AND BROTHERS,YADAV AND BROTHERS,YADAV AND BROTHERS,YADAV BRICK FIELD,YADAV BRICK FIELD,YADAV BRICK FIELD,YADAV BRICK FIELD,YADAV BRICKS FIELD,YADAV BRICKS FIELD,YADAV BRICKS FIELD,YADAV BRICKS FIELD,YADAV BROTHERS BRICKS FIELD,YADAV BROTHERS BRICKS FIELD,YADAV BROTHERS BRICKS FIELD,YADAV BROTHERS BRICKS FIELD,YADAV BUILDING MATERIALS,YADAV ENT BHATTHA,YADAV TRADERS,YASH PHARMA,YASH TRADERS,YASH TRADERS</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>EXCEL ENTERPRISES,EXCEL ENTERPRISES,EXCEL ENTERPRISES</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>GANESH UDYOG,GANESH UDYOG,GANESH UDYOG,GANESH UDYOG,GANGESH TRADERS,GANPATI MOBILE SERVICES,GANPATI TRADERS,GANPATI TRADERS,GAOURI SHANKER PRASAD &amp; JEYELLRS,GARG BAG HOUSE,GARG BAG HOUSE,GARG BAG HOUSE,GARG HOSIARY,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR PRASAD  AND SANTOSH KUMAR JEWELLERS,GAURI SHANKER PRASAD &amp; JEWLLERS,GAURI SHANKER PRASAD &amp; JEWLLERS,GAURI SHANKER PRASAD &amp; JEWLLERS,GAUTAM  ENTERPRISES,GAUTAM &amp; SONS,GAUTAM INTERNATIONAL,GAUTAM INTERNATIONAL,GAUTAM INTERNATIONAL,GAUTAM INTERNATIONAL,GAUTAM RICE AND FLOOR MILL,GAUTAM SALES,GAUTAM SALES,GAYTRI TRADERS,GAYTRI TRADERS,GAYTRI TRADERS,GAYTRI TRADERS,GEETA TRADERS,GEETA TRADERS,GEETA TRADERS,GHANASHYAM BRICKS FIELD,GHANSHYAM DAS SARRAF,GHANSHYAM DAS SARRAF,GHANSHYAM DAS SARRAF,GHANSHYAM DAS SARRAF,GHANSHYAM DAS SARRAF,GITA BRICKS FIELD,GITA BRICKS FIELD,GITA BRICKS FIELD,GOKUL MISHTHAN,GOPAL AGRO INDUSTRIES,GOPAL AGRO INDUSTRIES,GOPAL TRADERS,GOPAL TRADERS,GOPAL TRADERS,GORAKHPUR ELECTRIC WORKS,GOSWAMI KHAD BHANDA,GOVIND BRICK FIELD,GOVIND BRICK FIELD,GOVIND BRICK FIELD,GOVIND BRICK FIELD,GULAB SINGH,GUPTA &amp; COMPANY,GUPTA TRADERS,GUPTA TRADERS,GUPTA TRADERS,GUPTA TRADING COMPANY,GURU NANAK CYCLE STORE,GURU TRADERS,GURU TRADERS,GURU URVARK KENDAR,GURUKRIPA ENTERPRISES,GURUKRIPA ENTERPRISES,GYAN DUTT INTERPRISES,GYAN SINGH,GYAN SINGH,GYAN SINGH,GYAN SINGH,GYAN SINGH,GYAN SINGH,GYAN SINGH,GUPTA METAL STORES</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>THAKUR PRASAD JWLLERS,THE  MAQBOOL STATIONERY STORES,THE  MAQBOOL STATIONERY STORES,TIRUPATI TRADERS,TRIPATHI TRADERS,TULASI ASSOCIATES,T.N.L.F. TRADERS</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>VAIBHAV JWELLARS,VAIBHAV JWELLARS,VAISHNO DEVI RICE MILL,VANDE MATRAM,VICTORYAS FASHION,VIDHAN BRICKS FIELD,VIDHAN BRICKS FIELD,VIDHAN BRICKS FIELD,VIDHAN BRICKS FIELD,VIDHAN BRICKS FIELD,VIJAY AUTO MOBILES,VIJAY ELECTRICALS,VIJAY ELECTRICALS,VIJAY LAXMI ENT UDYOG,VIJAY LAXMI ENT UDYOG,VIJAY LAXMI ENT UDYOG,VIJAY LAXMI ENT UDYOG,VIJAY LAXMI ENT UDYOG,VIKAS ELECTRONICS,VIKASH ENTERPRISES,VIMAL AGRO INDUSTRIES,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY FURNITURE,VINAY TRADING COMPANY,VINOD KUMAR,VINOD KUMAR,VISHAL ENTERPRISES,VISHAL ENTERPRISES,VISHAWKARMA ELECTRIC WORKS,VISHAWKARMA ELECTRIC WORKS,VISHAWNATH TRADERS,VISHAWNATH TRADERS,VISHAWNATH TRADERS,VISHWA NATH SINGH B.K.O.,VISHWA NATH SINGH B.K.O.,VISHWA NATH SINGH B.K.O.,VISHWA NATH SINGH B.K.O.,VITECH IT SOLUTIONS,VITECH IT SOLUTIONS,Vineet kumar singh</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Firm Name,FASHION CLUB GARMENTS,FASHION CLUB GARMENTS,FINE ENTERPRISES,FINE HYDRAULIC WORKS,FINE HYDRAULIC WORKS,FRIENDS MOBILE</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>U.P.CONSTRUCTION ANDSUPPLIER,U.P.CONSTRUCTION ANDSUPPLIER,UJJWAL  ENTERPRISES,UMESH SHAHI,UMESH YADAV,UNITED EANGINEERS AND FABRICATERS,UNITED EANGINEERS AND FABRICATERS,UNITED EANGINEERS AND FABRICATERS,UTKARSH TRADING COMPANY</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
     <t>AADI SHAKTI TRADERS,AMAR TRADERS,AMRENDRA SHAHI,ANGEL COLLECTION,ANOOP GENERAL STORES,ANSARI RICE MILL,ANSH CONSTRUCTION,ANSH TELECOM,ANUPRIYA TRADERS,ATUL ENTERPRISES,ATUL VASTRAYALAY,A S TRADERS,A S TRADERS,A.B. CONSTRUCTION COMPNY,A.K.ELECTRONICS,A.K.S.BRICKS FIELD,A.K.S.BRICKS FIELD,A.M.S BRICKS FIELD,A.M.S BRICKS FIELD,A.P.S BRICKS FIELD,A.P.S BRICKS FIELD,A.P.S BRICKS FIELD,A.P.S BRICKS FIELD,A.P.S BRICKS FIELD,A.R.T.BRICKS FIELD,A.R.T.BRICKS FIELD,A.R.T.BRICKS FIELD,A.R.T.BRICKS FIELD,A.R.T.BRICKS FIELD,A.R.T.BRICKS FIELD,A.R.T.BRICKS FIELD,AANSH TRADERS,AANSH TRADERS,ABHISHEK GENERAL STORE,ABHISHEK GENERAL STORE,ABHISHEK GENERAL STORE,ABHISHEK TRADERS,ABHISHEK TRADERS,ADARSH ENTERPRISES,AJAY HARDWARE,AJAY INTERPRISES,AJAY KIRANA STORES,AJAY KUMAR OJHA,AJAY KUMAR RAJESH KUMAR,AJAY KUMAR RAJESH KUMAR,AJAY KUMAR RAJESH KUMAR,AJAY KUMAR RAJESH KUMAR,AJAY KUMAR SADHWANI B.K.O.,AJAY KUMAR SADHWANI B.K.O.,AJAY KUMAR SADHWANI B.K.O.,AJAY KUMAR VIJAY KUMAR,AJAY KUMAR VIJAY KUMAR,AKASH MOBILE,AKASH MOBILE,AKASH RICE MILL,ALAM FASHION WORLD,ALOK TRADERS,AMAN PALACE,AMAN SHAMIYANA HOUSE,AMAR CROCKERY CENTRE,AMAR CROCKERY CENTRE,AMAR GAS AGENCY,AMBEY PLY GLASS AND HARDWARE STORS,AMBEY TRADERS,AMBIKA ELECTRICALS,AMIT BRICKS FIELD,AMIT BRICKS FIELD,AMIT BRICKS FIELD,AMIT BRICKS FIELD,AMIT BRICKS FIELD,AMIT BRICKS FIELD,AMIT BRICKS FIELD,AMIT BRICKS FIELD,AMIT BRICKS FIELD,AMIT BRICKS FIELD,AMIT BRICKS FIELD,AMITDEEP AUTOMOBILES,ANAS TRADERS,ANIL VASTRALAY &amp; READYMADE GARMENTS,ANKIT SALES CORPORATION,ANKITA AGRO,ANKUR UDHYAM,ANKUR UDHYAM,ANNAPURNA INDUSTRIES,ANOOP KUMAR SINGH INT BHATTA,ANOOP KUMAR SINGH INT BHATTA,ANOOP KUMAR SINGH INT BHATTA,ANOOP KUMAR SINGH INT BHATTA,ANOOP KUMAR SINGH INT BHATTA,ANSHIKA BRICK FIELD,ANSHIKA BRICK FIELD,ANUBHAW ENTERPRISES,ANUJ BUILDERS,APOORVA JWELLARY HOUSE,ARIBA FOOT WEAR,ARIBA FOOT WEAR,ARIBA FOOT WEAR,ARIBA FOOT WEAR,ARIBA FOOT WEAR,ARIBA FOOT WEAR,ARVIND KUMAR SINGH,ARVIND SINGH,ASHISH FERTILIZER CENTER,ASHISH KUMAR AMIT KUMAR JEWELLERS,ASHISH KUMAR SANTOSH KUMAR JEWELLERS,ASHUTOSH TRADERS,ASHWANI HARDWARE,ATHENG ENGINEERING PRIVATE LIMITED,AVINASH BRICKS FIELD,AVINASH BRICKS FIELD,AVINASH BRICKS FIELD,AVINASH BRICKS FIELD,AWANTIKA ENTERPRISES,AWANTIKA ENTERPRISES,AWANTIKA ENTERPRISES,AWANTIKA ENTERPRISES,AYUSH JWELLERS,AYUSH TELECOM,AYUSH TELECOM,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADARSH BRICKS FIELD,ADITYA ASSOCIATES,ADITYA ASSOCIATES,AGARWAL TRADERS,AGARWAL TRADERS,APURVA SWEETS AND RESTAURANT,Arati Trunk House and alamira corner,ASHISH KUMAR ARUN KUMAR JEWELLERS,ASHOK TIVARI S/O SATYADEV TIVARI,ASHOK TIVARI S/O SATYADEV TIVARI,AYODHYA PRASHAD JAISHWAL S/O SHREE GANGADEEN</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>CHANDAN TRADERS,CHANDAN TRADERS,C.K.C  BRIKS  FIELD,C.K.C  BRIKS  FIELD,C.K.C  BRIKS  FIELD,CEMENT TRADERS,CHAND BRICKS FIELD,CHAND BRICKS FIELD,CHAND BRICKS FIELD,CHAND BRICKS FIELD,CHANDAN TRADERS,CHATURTH BHRATA STORES,CHAUDHARY VASTRALYA,CHAUHAN ENT UDYOG,CHAUHAN ENT UDYOG,CHAUHAN ENT UDYOG,CHAUHAN ENT UDYOG,CHAUHAN ENT UDYOG,CHAUHAN ENT UDYOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAUHAN INT UDOG,CHAURASIA BROTHERS,CHAURASIA BROTHERS,CHIRAG AGENCIES,CHIRAG AGENCIES,CHIRAG AGENCIES,CHIRAG AGENCIES,CHIRAG AGENCIES,CHOTE LAL DHIRAJ KUMAR SARRAF,CHOTE LAL DHIRAJ KUMAR SARRAF,CIELO SEWING MACHINE COMPANY,COOL BREEZE SERVICES,COOL BREEZE SERVICES</t>
+    <t>B</t>
+  </si>
+  <si>
+    <t>BABA PASHU AAHAR,BABA BRICKS FIELD,BABA BRICKS FIELD,BABA BRICKS FIELD,BABA BRICKS FIELD,BABA BRICKS FIELD,BABA GORAKHNATH IRON STORES,BABA JI MORDEN RICE MILL,BABA JI MORDEN RICE MILL,BABA MAHARAJ JI BRICK FIELD,BABA MAHARAJ JI BRICK FIELD,BABLU SINGH BUILDING  MATERIAL,BAIJNATH TRADERS,BAIJNATH TRADERS,BAJAJ BROTHERS,BAJRA SHAKTI IT BHATHA,BAJRA SHAKTI IT BHATHA,BAJRA SHAKTI IT BHATHA,BAJRANG BRICKS FIELD,BAJRANG BULLION TRADERS,BALA JI ENTERPRISES,BALAJI TRADERS,BALAJI TRADERS,BALVANT YADAV PLUMBRING WORKS,BALWANT SINGH BRICK FIELD,BALWANT SINGH BRICK FIELD,BALWANT SINGH BRICK FIELD,BALWANT SINGH BRICK FIELD,BALWANT SINGH BRICK FIELD,BHARAT PLASTIC,BHOLA HOSIERY,BISHESH TRADING COMPANY,BISWAS TRADERS,BISWAS TRADERS,BISWAS TRADERS,BOL BUM CONSTRUCTION,BOMBAY SURGICAL,BOMBAY SURGICAL,BOMBAY SURGICAL,BRIJMOHAN JAISWAL,BULLIAN TRADERS,BULLIAN TRADERS</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>DEEPAK TENT HOUSE,DINESH SINGH KHADI BHANDAR,D.B.SONS,D.K.TRADERS,D.K.TRADERS,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DANISH  LARI CEMENT SUPPLIER,DAS AGENCIES,DEENA NATH SINGH  B.K.O,DEENA NATH SINGH  B.K.O,DEENA NATH SINGH  B.K.O,DEENA NATH SINGH  B.K.O,DEEPAK ASSOCIATE,DEEPAK ASSOCIATE,DEEPAK ASSOCIATE,DEEPAK AUZAR BHANDAR,DHIRAJ AUTOMOBILES,DHOODHNATH GUPTA CEMENT AGENCY,DIGVIJAI SINGH ENT BHATTA,DIGVIJAI SINGH ENT BHATTA,DIGVIJAI SINGH ENT BHATTA,DILIP SINGH,DILIP SINGH,DILIP SINGH,DREAM ENTERPRISES,DURGA TRADERS,DURGA TRADERS,DURGESH ENGINEERING,DEVA BRICKS FIELD,DEVA BRICKS FIELD,DEVA BRICKS FIELD,DEVA BRICKS FIELD,DIGVIJAY SINGH ENT BHATTA,DIGVIJAY SINGH ENT BHATTA,DIGVIJAY SINGH ENT BHATTA,DIGVIJAY SINGH ENT BHATTA</t>
   </si>
   <si>
     <t>O</t>
@@ -36,28 +114,28 @@
     <t>OM SHRI SAI TRADERS,OEM METAL CAP INDUSTRIES,OEM METAL CAP INDUSTRIES,OEM METAL CAP INDUSTRIES,OM  ENTERPRISES,OM BRICKS FIELD,OM BRICKS FIELD,OM BRICKS FIELD,OM BRICKS UDHYOG,OM FURNITURE,OM GARMENTS AND FOOTWEAR,OM PHARMACEUTICALS,OM PHARMACEUTICALS,OM PLASTIC,OM PLASTIC,OM PLASTIC,OM PRAKASH KIRANA STORES,OM RICE MILL,OM SAI NATH ENTERPRISES,OM TRADERS,O.K.TRADERS</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>YASH ENTERPRISES,YASH GARMENT,YADAV AGENCY,YADAV AND BROTHERS,YADAV AND BROTHERS,YADAV AND BROTHERS,YADAV BRICK FIELD,YADAV BRICK FIELD,YADAV BRICK FIELD,YADAV BRICK FIELD,YADAV BRICKS FIELD,YADAV BRICKS FIELD,YADAV BRICKS FIELD,YADAV BRICKS FIELD,YADAV BROTHERS BRICKS FIELD,YADAV BROTHERS BRICKS FIELD,YADAV BROTHERS BRICKS FIELD,YADAV BROTHERS BRICKS FIELD,YADAV BUILDING MATERIALS,YADAV ENT BHATTHA,YADAV TRADERS,YASH PHARMA,YASH TRADERS,YASH TRADERS</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>EXCEL ENTERPRISES,EXCEL ENTERPRISES,EXCEL ENTERPRISES</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>U.P.CONSTRUCTION ANDSUPPLIER,U.P.CONSTRUCTION ANDSUPPLIER,UJJWAL  ENTERPRISES,UMESH SHAHI,UMESH YADAV,UNITED EANGINEERS AND FABRICATERS,UNITED EANGINEERS AND FABRICATERS,UNITED EANGINEERS AND FABRICATERS,UTKARSH TRADING COMPANY</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>VAIBHAV JWELLARS,VAIBHAV JWELLARS,VAISHNO DEVI RICE MILL,VANDE MATRAM,VICTORYAS FASHION,VIDHAN BRICKS FIELD,VIDHAN BRICKS FIELD,VIDHAN BRICKS FIELD,VIDHAN BRICKS FIELD,VIDHAN BRICKS FIELD,VIJAY AUTO MOBILES,VIJAY ELECTRICALS,VIJAY ELECTRICALS,VIJAY LAXMI ENT UDYOG,VIJAY LAXMI ENT UDYOG,VIJAY LAXMI ENT UDYOG,VIJAY LAXMI ENT UDYOG,VIJAY LAXMI ENT UDYOG,VIKAS ELECTRONICS,VIKASH ENTERPRISES,VIMAL AGRO INDUSTRIES,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY  BRICKS FIELD,VINAY FURNITURE,VINAY TRADING COMPANY,VINOD KUMAR,VINOD KUMAR,VISHAL ENTERPRISES,VISHAL ENTERPRISES,VISHAWKARMA ELECTRIC WORKS,VISHAWKARMA ELECTRIC WORKS,VISHAWNATH TRADERS,VISHAWNATH TRADERS,VISHAWNATH TRADERS,VISHWA NATH SINGH B.K.O.,VISHWA NATH SINGH B.K.O.,VISHWA NATH SINGH B.K.O.,VISHWA NATH SINGH B.K.O.,VITECH IT SOLUTIONS,VITECH IT SOLUTIONS,Vineet kumar singh</t>
+    <t>P</t>
+  </si>
+  <si>
+    <t>P Y S TRADERS,PANDEY ENTERPRISES,PRAJAPATI TRADERS,PRAKASH TRADERS,PRATAP BRICKS FIELD,PRATAP BRICKS FIELD,PRATAP BRICKS FIELD,PURETY FOAMS,PURNESHWARI ENTERPRISES,PADMAKAR  TRIPATHI,PAINT HOUSE,PAINT HOUSE,PAINT HOUSE,PANDEY PUSTAK MANDIR,PANDEY TRADERS,PANDEY TRADERS,PANJ SPORTS,PANJTAN SPORTS,PANKAJ BRICKS FIELD,PANKAJ BRICKS FIELD,PANKAJ BRICKS FIELD,PANKAJ BRICKS FIELD,PANKAJ BRICKS FIELD,PARMESHWAR FLOOR MILL,PARMESHWAR FLOOR MILL,PARMESHWAR FLOOR MILL,PARMESHWAR FLOOR MILL,PAWAN AGRO AGENCY,PAWAN BRICK FIELD,PAWAN BRICK FIELD,PAWAN BRICK FIELD,PAWAN BRICK FIELD,PAWAN FURNITURE UDHYOUG,PAWAN FURNITURE UDHYOUG,PAWAN FURNITURE UDHYOUG,PAWAN KHAD BHANDAR,PAYAL JEWELLERS,PJD BRICK FIELD,PJD BRICK FIELD,PJD BRICK FIELD,PRABHAW  MOBILE AND REPAIRING CENTER,PRABHUNATH TRADERS,PRADEEP KUMAR HANUMAN PRASAD TRADERS,PRAGYA ELECTRIC &amp; ELECTRONICS,PRAGYA ENTERPRISES,PRAKASH SOLAR SHOP,PRAMILLA TRADERS,PRAMILLA TRADERS,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM PRAKASH &amp; CO.,PREM PRAKASH &amp; CO.,PREM PRAKASH &amp; CO.,PREM SHANKAR PASWAN,PREMA CONSTRUCTION,,PREMA CONSTRUCTION,,PREMA CONSTRUCTION,,PRIYAM TRADERS,PUJA BRICKS FIELD,PUJA BRICKS FIELD,PUJA BRICKS FIELD,PUJA BRICKS FIELD,PUNJAB AGRO SALES,PUNJAB ELECTRICALS,PURUSHOTTAM JEWELLERY HOUSE PVT.LTD.,PURVANCHAL ASSOCIATES,PURVANCHAL ELECTRICALS STORES,PURVANCHAL FOODS,PAWAN TRADERS,PAWAN TRADERS,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R. K. PLASTIC UDYOG,R. R. BROTHERS,R. R. BROTHERS,RADHA BRICKS UNIT,RAI AUTOMOBILE,RAI AUTOMOBILE,RAI AUTOMOBILE,RAI TRADERS,RAJ TRADERS,RAJESH ELECTRONCS AND MOBILE SHOP,RASMUNI AGENCIES,R.K.BRICKS FIELD,R.K.BRICKS FIELD,R.K.BRICKS FIELD,R.K.T.K.TRADERS,R.N. BRICKS FIELD,R.N. BRICKS FIELD,R.N. BRICKS FIELD,R.N.ENTERPRISES,R.P. BRIKS FILD,R.P. BRIKS FILD,R.P. BRIKS FILD,R.P. BRIKS FILD,R.P. BRIKS FILD,R.P. BRIKS FILD,R.S. ENTER PRISES,R.S.MARKETING &amp; COMPANY,R.S.MARKETING &amp; COMPANY,R.S.MARKETING &amp; COMPANY,RAHUL BRICKS FIELD,RAHUL BRICKS FIELD,RAHUL BRICKS FIELD,RAHUL BRICKS FIELD,RAHUL BRICKS FIELD,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAJ AGENCIES,RAJ AGENCIES,RAJ TRADERS,RAJ TRADERS,RAJ TRADERS,RAJENDRA ENTERPRISES,RAJENDRA TRADERS,RAJESH GOEL JWELLERS,RAJESH JEWLLERS,RAJESH KUMAR SANJAY KUMAR,RAJESH KUMAR SANJAY KUMAR,RAJESHWAR KUMAR YADAV,RAJVEER CONSTRUCTION,RAM BELAS,RAM CHANDRA SURRAF,RAM CHANDRA SURRAF,RAM JI SUNIL KUMAR JEWELLERS,RAM KARAN YADAV GOVT CONTRACTOR AND SUPPLYER,RAM KUMAR SINGH,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM PRASAD SUNIL KUMAR SARAF,RAMESH BRICKS FIELD,RAMESH BRICKS FIELD,RAMESH BRICKS FIELD,RAMESH BRICKS FIELD,RAMESH BRICKS FIELD,RAMUJAGIR TIWARI,RAVI PRATAP YADAV B.K.O.,RAVI PRATAP YADAV B.K.O.,RAVINDRA PRATAP SINGH B.K.O,RAVINDRA PRATAP SINGH B.K.O,RAVINDRA PRATAP SINGH B.K.O,RAVINDRA PRATAP SINGH B.K.O,RAVINDRA PRATAP SINGH B.K.O,RICHA H P GAS GRAMIN  VITARAK,RICHA H P GAS GRAMIN  VITARAK,RISHABH TRADERS,RISHI DRESSES,ROCKY MEDICAL STORES,ROCKY MEDICAL STORES,ROCKY MEDICAL STORES,ROSHNI ENTERPRISES,RAJEEV COMMUNICATION AND MOTORS,RAM CHANDER SWEET</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>IDIAL ENTERPRISES,INDIA  CEMENT STORE,INDIA  CEMENT STORE,INDIA CYCLE COMPANY,INDIA CYCLE COMPANY,INDIA CYCLE TRADING COMPANY,ISHAN  DXN HEALTH CARE</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>jai ambey traders</t>
   </si>
   <si>
     <t>s</t>
@@ -66,16 +144,10 @@
     <t>shivam brick fild</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Firm Name,FASHION CLUB GARMENTS,FASHION CLUB GARMENTS,FINE ENTERPRISES,FINE HYDRAULIC WORKS,FINE HYDRAULIC WORKS,FRIENDS MOBILE</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>K D ENTERPRISES,KASAUDHAN JEWELLERS,KISHORI LAL SURENDRA KUMAR SARRAF,K G N TRADERS,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K. P. SINGH  ENT  BHATTA,K.C.Y.  MARKA INT BHATTHA,K.C.Y.  MARKA INT BHATTHA,K.S.K.,K.S.K.,K.S.K.,KAILASH HOSIERY,KAILASH HOSIERY,KAMAZ VECTRA MOTORS LTD.,KAMAZ VECTRA MOTORS LTD.,KAMAZ VECTRA MOTORS LTD.,KANAK JEWELLERS,KANAK JEWELLERS,KANCHAN MOBILE WORLD,KANCHAN MOBILE WORLD,KANCHAN MOBILE WORLD,KANHA JEWELLERS,KANHA JEWELLERS,KANHAIYA GENERAL STORE,KAPIL DEV BRICKS FIELD,KAPIL DEV BRICKS FIELD,KASAUDHAN TRADERS,KATWARU SARAF AND CO.,KEDIA HOSIERY,KESHAV HOSIERY,KESHAV HOSIERY,KESHAV HOSIERY,KISAN EINT BHATTA,KISAN EINT BHATTA,KISAN EINT BHATTA,KISAN KHAD BHANDAR,KISAN SEWA KENDRA,KISAN SEWA KENDRA,KISAN SEWA KENDRA,KISAN SEWA KENDRA,KISHAN URVARAK KENDRA,KISHAN URVARAK KENDRA,KRISH ENTERPRISES,KRISHAK SEWA KENDRA,KRISHANKANT  INDANE GRAMIN VITARAK,KRISHANKANT  INDANE GRAMIN VITARAK,KRISHI SEWA KENDRA,KRISHI SEWA KENDRA,KRISHNA BIHARI LAL JWELLERS PVT.LTD.,KRISHNA BIHARI LAL JWELLERS PVT.LTD.,KRISHNA BRICKS FIELD,KRISHNA BRICKS FIELD,KRISHNA BRICKS FIELD,KRISHNA BRICKS FIELD,KRISHNA PACKAGING SOLUTION,KRISHNA PACKAGING SOLUTION,KRISHNA READYMADE CENTER,KRISHNA READYMADE CENTER,KUMAR AGENCIES,KUMAR AGENCIES,KUMAR TRADING CO,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,KUNAL BRICKS FIELD,K.K. BRICKS FIELD,K.K. BRICKS FIELD,K.K. BRICKS FIELD,Krishna Feling Station,Krishna Feling Station</t>
+    <t>M</t>
+  </si>
+  <si>
+    <t>M.D. FAMILY SHOP,MAA SARYU ENTERPRISES AND OTHERS,MAHA LAXMI TEXTILES,MAHA LAXMI TEXTILES,M.B. NARAYAN,M.G.COPY MANUFACTURING UNIT,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA BRICKS FIELD,MAA BRICKS FIELD,MAA BRICKS FIELD,MAA BRICKS FIELD,MAA CONSTRUCTION,MAA DURGA RICE MILL,MAA EENT UDYOG,MAA GAURI ASSOCIATES,MAA GAURI ASSOCIATES,MAA SAMAY BRICK FIELD,MAA SAMAY BRICK FIELD,MAA SAMAY BRICK FIELD,MAA SAMAY BRICK FIELD,MAA SAMAY BRICK FIELD,MAA SAMAY BRICK FIELD,MAA SAMAY BRICKS FIELD,MAA SAMAY BRICKS FIELD,MAA SHARDA AUTO MOBILE,MAA SHARDA AUTO MOBILE,MAA SHARDA PHARMA,MAA VAISHNO AUTOMOBILES,MAA VAISHNO AUTOMOBILES,MAA VAISHNO ENTERPRISES,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO MINI RICE MILL,MAA VAISHNO OIL AGENCY,MAA VAISHNO OIL AGENCY,MAA VAISHNO OIL AGENCY,MAA VAISHNO OIL AGENCY,MAA VAISHNO TRADERS,MAA VAISHNO TRADING COPMANY,MAA VAISHNO TRADRS,MAA VASHNO TRADERS,MAA VASHNO TRADERS,MADANESHWAR CHAND BKO.,MADANESHWAR CHAND BKO.,MADDHESIYA RICE MILL,MADHAV ENTERPRISES,MADHESHIYA RICE MILL,MADHESHIYA RICE MILL,MADHESHIYA RICE MILL,MADHESHIYA RICE MILL,MADHESIYA PACKING INDUSTRIES,MAHA LAXMI,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAK INTERPRISES,MAMATA AUTO MOBILS,MANISH TRADERS,MANISH TRADERS,MANISH TRADERS,MANOJ BRICKS FIELD,MANOJ BRICKS FIELD,MANOJ BRICKS FIELD,MANOJ BUILDING MATERIAL AND HARDWARE,MANOJ OPTICALS,MEERA DEVI,MEERA DEVI,MEERA DEVI,MEERA DEVI,MIRZA &amp; SONS,MIRZA &amp; SONS,MIRZA &amp; SONS,MISHRA INT UDYOG,MISHRA INT UDYOG,MISHRA INT UDYOG,MISHRA INT UDYOG,MISHRA INT UDYOG,MUNNA MOBILE SHOP,MURLI ENT BHATTHA UDYOG,MURLI ENT BHATTHA UDYOG,MURLI ENT BHATTHA UDYOG,MURLI ENT BHATTHA UDYOG,MURLI ENT BHATTHA UDYOG,MURLI ENTERPRISES,MAA AMBEY MARKETING AGENCY,MAA AMBEY MARKETING AGENCY,Mohd. Usman s/o Mohd. usuf</t>
   </si>
   <si>
     <t>N</t>
@@ -84,82 +156,10 @@
     <t>NEW GOVIND BRICKS FIELD,NEW GOVIND BRICKS FIELD,NEW GOVIND BRICKS FIELD,NEW VERMA JEWELLERS,NIGAM BARTAN STORES,NITIN OPTICALAS,N.K.AGENCY,NAGESH TRIPATHI THIKEDAR,NANAK TRADERS,NANAK TRADERS,NAND BUILDING MATARIALS,NARAYAN BRICKS FIELD,NARAYAN BRICKS FIELD,NARAYAN BRICKS FIELD,NARAYAN BRICKS FIELD,NATIONAL AGENCY,NATIONAL AGENCY,NATIONAL SERVICES,NATIONAL SERVICES,NATIONAL TRADERS,NAV BHARAT CONSTRUCTION,NEHA ELECTRONICS  AND  ELECTRICALS,NEW ASHISH AGENCY,NEW KAILASH HOSIERY,NEW KAILASH HOSIERY,NEW MAHAVEER ENT BHATTHA,NEW MAHAVEER ENT BHATTHA,NEW MAHAVEER ENT BHATTHA,NEW MAHAVEER ENT BHATTHA,NEW MAHAVEER ENT BHATTHA,NEW MAHAVEER ENT BHATTHA,NEW NATIONAL CHEMICAL TRADERS,NEW NATIONAL CHEMICAL TRADERS,NEW NATIONAL FOOTWEAR,NEW PANDEY BRICKS FIELD,NEW PANDEY BRICKS FIELD,NEW PANDEY BRICKS FIELD,NEW PANDEY BRICKS FIELD,NEW PANDEY BRICKS FIELD,NEW PANDEY BRICKS FIELD,NEW RAVI JALPAAN GRIH,NEW RUCHIKA HOSIERY</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>P Y S TRADERS,PANDEY ENTERPRISES,PRAJAPATI TRADERS,PRAKASH TRADERS,PRATAP BRICKS FIELD,PRATAP BRICKS FIELD,PRATAP BRICKS FIELD,PURETY FOAMS,PURNESHWARI ENTERPRISES,PADMAKAR  TRIPATHI,PAINT HOUSE,PAINT HOUSE,PAINT HOUSE,PANDEY PUSTAK MANDIR,PANDEY TRADERS,PANDEY TRADERS,PANJ SPORTS,PANJTAN SPORTS,PANKAJ BRICKS FIELD,PANKAJ BRICKS FIELD,PANKAJ BRICKS FIELD,PANKAJ BRICKS FIELD,PANKAJ BRICKS FIELD,PARMESHWAR FLOOR MILL,PARMESHWAR FLOOR MILL,PARMESHWAR FLOOR MILL,PARMESHWAR FLOOR MILL,PAWAN AGRO AGENCY,PAWAN BRICK FIELD,PAWAN BRICK FIELD,PAWAN BRICK FIELD,PAWAN BRICK FIELD,PAWAN FURNITURE UDHYOUG,PAWAN FURNITURE UDHYOUG,PAWAN FURNITURE UDHYOUG,PAWAN KHAD BHANDAR,PAYAL JEWELLERS,PJD BRICK FIELD,PJD BRICK FIELD,PJD BRICK FIELD,PRABHAW  MOBILE AND REPAIRING CENTER,PRABHUNATH TRADERS,PRADEEP KUMAR HANUMAN PRASAD TRADERS,PRAGYA ELECTRIC &amp; ELECTRONICS,PRAGYA ENTERPRISES,PRAKASH SOLAR SHOP,PRAMILLA TRADERS,PRAMILLA TRADERS,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM ENTERPRISES,PREM PRAKASH &amp; CO.,PREM PRAKASH &amp; CO.,PREM PRAKASH &amp; CO.,PREM SHANKAR PASWAN,PREMA CONSTRUCTION,,PREMA CONSTRUCTION,,PREMA CONSTRUCTION,,PRIYAM TRADERS,PUJA BRICKS FIELD,PUJA BRICKS FIELD,PUJA BRICKS FIELD,PUJA BRICKS FIELD,PUNJAB AGRO SALES,PUNJAB ELECTRICALS,PURUSHOTTAM JEWELLERY HOUSE PVT.LTD.,PURVANCHAL ASSOCIATES,PURVANCHAL ELECTRICALS STORES,PURVANCHAL FOODS,PAWAN TRADERS,PAWAN TRADERS,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD,PRTAP BRIKS FEALD</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>S S ENTERPRISES,S. K. TRADERS,SACHIN MINERAL WATER,SADBHAWANA ENTERPRISES,SADBHAWANA ENTERPRISES,SAI TREDERS,SAMINFRATECH INDIA,SANTOSHI TRADERS,SHANU ELECTRONICS,SHIV ENTERPRISES,SHREE AUTOMOBILES,SHRI DURGA ENTERPRISES,SHRI VAIBHAW STATIONERY AND ELECTRIC,SINGH BUILDING MATERIALS,SWARGIYA SHRI KANSHIRAM FOUNDATION,S K ENTERPRISES,S. ENTERPRISES,S.D. CHAURASIYA KIRANA STORE,S.D. CHAURASIYA KIRANA STORE,S.D. CHAURASIYA KIRANA STORE,S.K. ELECTRICALS,S.K. ENTERPRISES,S.K.JWELLERS,S.P. BRICKS FIELD,S.P. BRICKS FIELD,S.P. BRICKS FIELD,S.P. BRICKS FIELD,S.P. BRICKS FIELD,S.P. BRICKS FIELD,S.P. ENTERPRISES,S.P. ENTERPRISES,S.P. ENTERPRISES,S.S.CAITRERS,SADHU BRICKS FIELD,SAHANI CYCLE STORES,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAI BABA BRICKS FIELD,SAKSHI ENTERPRISES,SAM SPORTS,SANDEEP ENTERPRISES,SANDEEP HARDWARE &amp; PAINTS,SANGAM ENTERPRISES,SANGAM RICE MILL,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY BRICKS FIELD,SANJAY CHAND,SANJAY KUMAR GUPTA,SANJAY KUMAR GUPTA,SANTOSH COAL DIPO,SAR ENTERPRISES,SARASVATI TRADERS,SARASVATI TRADERS,SARASVATI TRADERS,SARASVATI TRADERS,SARASVATI TRADERS,SARASVATI TRADERS,SAROJ COMMUNICATION,SAROJ COMMUNICATION,SAROJ COMMUNICATION,SATNAM MACHINES,SATNAM MACHINES,SATNAM MACHINES,SATNAM MACHINES,SATNAM MACHINES,SATNAM MACHINES,SATNAM MACHINES,SATYA ENTERPRISES,SHAHEED J.K.TRIPATHI AUTOMOBILES,SHAHEED J.K.TRIPATHI AUTOMOBILES,SHAHID J.K.TRIPATHI AUTO MOBILES,SHAIVVI TRADERS,SHAKTI INT UDHOGH,SHAKTI INT UDHOGH,SHAKUNTALA   JWELLERS,SHAKUNTALA   JWELLERS,SHANKAR AUTO  MOBILES,SHANKAR AUTO  MOBILES,SHANKAR AUTO  MOBILES,SHANKAR AUTO  MOBILES,SHARDA TRADERS,SHARDA TRADERS,SHARDA TRADERS,SHAREEF DUPATTA PALACE,SHEKHAR TRADERS,SHIBLEE  TRADERS,SHIBLEE  TRADERS,SHIBLEE ENTERPRISES,SHIV AUTO SALES,SHIV SHAKTI BRICKS FIELD,SHIV SHAKTI ENTERPRISES,SHIV SHAKTI ENTERPRISES,SHIV SHAKTI GALLA BHANDAR,SHIV SHAKTI MADERN RICE MILL,SHIV SHAKTI MADERN RICE MILL,SHIV SHAKTI TRADERS,SHIV SHAKTI TRADERS,SHIV SHAKTI TRADERS,SHIV SHAKTI TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIV TRADERS,SHIVA AGENCIES,SHIVA AGENCIES,SHIVA ENGINEERING STORE,SHIVA ENGINEERING STORE,SHIVA TRADERS,SHIVA TRADERS,SHIVA TRADERS,SHIVA TRADERS,SHIVA TRADERS,SHIVA TRADERS,SHIVAM ASSOCIATES,SHIVAM ASSOCIATES,SHIVAM ASSOCIATES,SHIVAM ENTERPRISES,SHIVAM ENTERPRISES,SHIVAM KIRANA STORE,SHIVAM TRADERS,SHIVAM TRADERS,SHIVESH JEWELLERS,SHRADHA ELECTRICAL &amp; ELECTRONICS,SHREE  SHYAM JWELLERS,SHREE BALAJI GARMENTS,SHREE BRICKS FIELD,SHREE JOYTI JEWELLERS,SHREE LAXMI GARMENTS,SHREE LAXMI GARMENTS,SHREE MAA SHEETALA JEWELLERS,SHREE MAHABIR  TRADING  COMPANY,SHREE MAHAKAL ASSOCIATES,SHREE PURSHOTTAM JEWELLERY HOUSE,SHREE SHREE  SAI NATH SWEET HOUSE,SHREE SHREE  SAI NATH SWEET HOUSE,SHREE SHREE  SAI NATH SWEET HOUSE,SHREE SHREE  SAI NATH SWEET HOUSE,SHRI DURGA GARMENTS,SHRI DURGA GARMENTS,SHRI HARI GARMENTS,SHRI JYOTI DHARMKANTA AND JEWLLERS,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI KRISHNA BRICK FIELD,SHRI LAXMI TRADING CO.,SHRI LAXMI TRADING CO.,SHRI LUXMI TRADERS,SHRI LUXMI TRADERS,SHRI LUXMI TRADERS,SHRI NAV DURGA TRADING COMPANY,SHRI VIGHNESHWAR STEELS AND HARDWARE CENTER,SHYAM ENTERPRISES,SHYAM SUNDAR MANISH KUMAR SARRAF,SHYAMENDRA SHAHI,SINGH AUTOMOBILES,SINGH AUTOMOBILES,SINGH AUTOMOBILES,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH BRICKS FILED,SINGH ENT BHATTHA,SINGH ENT BHATTHA,SINGH ENT BHATTHA,SINGH MEDICAL STORE,SINGH MEDICAL STORE,SINGH TRADERS,SINGH TRADERS,SINGH TRADERS,SINGH TRADERS,SITA RAM GANESH PRASAD SARAF,SITA RAM GANESH PRASAD SARAF,SONBARSA BRICKS FIELD,SONBARSA BRICKS FIELD,SONBARSA BRICKS FIELD,SREE RAPTI TRADERS,SRI  BALAJI JEWELLERS,SRI AMBEY  JEWELLERS,SRI AMBEY  JEWELLERS,SRI BALAJI AUTO SALES,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI KRISHNA TRADERS,SRI SAI TRADING COMPANY,SRI SATYAM GARMENTS,SRI SATYAM GARMENTS,SRI SHANKER ENTERPRISES,STAR BAG HOUSE,STAR HANDLOOM AND HOSIERY SALE,STAR HANDLOOM AND HOSIERY SALE,STAR REFRIGERATION,SUBHAM DISTRIBUTORS,SUBHAM DISTRIBUTORS,SUBHAS BUILDING MATERIALS,SUBHASH MEDICAL STORES,SUDAMA BHARAT GAS GRAMIN VITRAK,SUDAMA BHARAT GAS GRAMIN VITRAK,SUNIL JWELLERS,SUNNY ELECTRONICS,SUNNY ELECTRONICS,SUNNY ELECTRONICS,SUNNY ELECTRONICS,SUNNY ELECTRONICS,SUPER STONE CRUSHER,SUPER STONE CRUSHER,SURAJ BEEJ BHANDAR,SURAJ ENTERPRISES,SURYANSH CONSTRUCTION &amp; SUPPLIERS,SUSHIL ENTERPRISES,SUSHIL ENTERPRISES,SUSHIL ENTERPRISES,SUSHIL ENTERPRISES,SUSHIL KUMAR MANISH KUMAR SARRAF,SUSHIL KUMAR MANISH KUMAR SARRAF,SWYANGAR ASSOCIATES,SWYANGAR ASSOCIATES,SWYANGAR ASSOCIATES,S.P.TRADERS,SANJAI PLASTIC TRADERS,SANJAI PLASTIC TRADERS</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>GANESH UDYOG,GANESH UDYOG,GANESH UDYOG,GANESH UDYOG,GANGESH TRADERS,GANPATI MOBILE SERVICES,GANPATI TRADERS,GANPATI TRADERS,GAOURI SHANKER PRASAD &amp; JEYELLRS,GARG BAG HOUSE,GARG BAG HOUSE,GARG BAG HOUSE,GARG HOSIARY,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR ENT BHATTA,GAURI SHANKAR PRASAD  AND SANTOSH KUMAR JEWELLERS,GAURI SHANKER PRASAD &amp; JEWLLERS,GAURI SHANKER PRASAD &amp; JEWLLERS,GAURI SHANKER PRASAD &amp; JEWLLERS,GAUTAM  ENTERPRISES,GAUTAM &amp; SONS,GAUTAM INTERNATIONAL,GAUTAM INTERNATIONAL,GAUTAM INTERNATIONAL,GAUTAM INTERNATIONAL,GAUTAM RICE AND FLOOR MILL,GAUTAM SALES,GAUTAM SALES,GAYTRI TRADERS,GAYTRI TRADERS,GAYTRI TRADERS,GAYTRI TRADERS,GEETA TRADERS,GEETA TRADERS,GEETA TRADERS,GHANASHYAM BRICKS FIELD,GHANSHYAM DAS SARRAF,GHANSHYAM DAS SARRAF,GHANSHYAM DAS SARRAF,GHANSHYAM DAS SARRAF,GHANSHYAM DAS SARRAF,GITA BRICKS FIELD,GITA BRICKS FIELD,GITA BRICKS FIELD,GOKUL MISHTHAN,GOPAL AGRO INDUSTRIES,GOPAL AGRO INDUSTRIES,GOPAL TRADERS,GOPAL TRADERS,GOPAL TRADERS,GORAKHPUR ELECTRIC WORKS,GOSWAMI KHAD BHANDA,GOVIND BRICK FIELD,GOVIND BRICK FIELD,GOVIND BRICK FIELD,GOVIND BRICK FIELD,GULAB SINGH,GUPTA &amp; COMPANY,GUPTA TRADERS,GUPTA TRADERS,GUPTA TRADERS,GUPTA TRADING COMPANY,GURU NANAK CYCLE STORE,GURU TRADERS,GURU TRADERS,GURU URVARK KENDAR,GURUKRIPA ENTERPRISES,GURUKRIPA ENTERPRISES,GYAN DUTT INTERPRISES,GYAN SINGH,GYAN SINGH,GYAN SINGH,GYAN SINGH,GYAN SINGH,GYAN SINGH,GYAN SINGH,GUPTA METAL STORES</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>jai ambey traders</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>DEEPAK TENT HOUSE,DINESH SINGH KHADI BHANDAR,D.B.SONS,D.K.TRADERS,D.K.TRADERS,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DADA BRICKS FIELD,DANISH  LARI CEMENT SUPPLIER,DAS AGENCIES,DEENA NATH SINGH  B.K.O,DEENA NATH SINGH  B.K.O,DEENA NATH SINGH  B.K.O,DEENA NATH SINGH  B.K.O,DEEPAK ASSOCIATE,DEEPAK ASSOCIATE,DEEPAK ASSOCIATE,DEEPAK AUZAR BHANDAR,DHIRAJ AUTOMOBILES,DHOODHNATH GUPTA CEMENT AGENCY,DIGVIJAI SINGH ENT BHATTA,DIGVIJAI SINGH ENT BHATTA,DIGVIJAI SINGH ENT BHATTA,DILIP SINGH,DILIP SINGH,DILIP SINGH,DREAM ENTERPRISES,DURGA TRADERS,DURGA TRADERS,DURGESH ENGINEERING,DEVA BRICKS FIELD,DEVA BRICKS FIELD,DEVA BRICKS FIELD,DEVA BRICKS FIELD,DIGVIJAY SINGH ENT BHATTA,DIGVIJAY SINGH ENT BHATTA,DIGVIJAY SINGH ENT BHATTA,DIGVIJAY SINGH ENT BHATTA</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>J. A. S.  BRICKS FILED,JAI MAA AMBEY TRADERS,JAI MAA AMBEY TRADERS,JAI MAA AMBEY TRADERS,JAI MAA VAISHNO TRADERS,JAI MATA DI KHAD BHANDAR,JAISWAL AUTO MOBILES,JAISWAL AUTO MOBILES,JAISWAL TRADERS,J.K.TRADERS,J.K.TRADERS,J.P. ENTERPRISES,J.P. ENTERPRISES,J.P. ENTERPRISES,J.P. ENTERPRISES,JAG GANGA SETH  JEWELLERS,JAGDAMBIKA FILLING STAION,JAGDISH  PRASAD,JAGMAG FIREWORKS,JAI AMBEY TRADING CO.,JAI AMBEY TRADING CO.,JAI AMBEY TRADING CO.,JAI MAA DURGE,JAI MAA KALI HARVESTERS,JAI MAA VAISHNO DEVI TRADERS,JAI MAA VASHNO TRADERS,JAI MAA VASHNO TRADERS,JAI MAA VASHNO TRADERS,JAI MAA VASHNO TRADERS,JAI PRAKASH SARAF AND COMPANY,JAI PRAKASH SARAF AND COMPANY,JAI SRI RAM HOSIERY,JAIPRAKASH CHAURASIA,JAISWAL BRICKS FIELD,JAISWAL BRICKS FIELD,JAISWAL BRICKS FIELD,JAISWAL BUILDING MATERIAL,JAISWAL BUILDING MATERIAL,JAISWAL MACHINARY,JAISWAL MACHINARY,JAISWAL MEDICAL STORES,JAISWAL MEDICAL STORES,JAISWAL TRADERS,JAISWAL TRADERS,JAISWAL TRADERS,JAISWAL TRADERS,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING CO.,JAISWAL TRADING COMPANY,JANATA HARDWARE CENTER,JANTA BUILDING MATERIALS,JANTA CIMENT STORES,JANTA TRADERS,JANTA TRADERS,JANTA TRADING CO.,JANTA TRADING CO.,JAWAHAR MEDICAL STORES,JAY CYCELS,JAYSWAL TRADERS,J.K.GARMENTS</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>IDIAL ENTERPRISES,INDIA  CEMENT STORE,INDIA  CEMENT STORE,INDIA CYCLE COMPANY,INDIA CYCLE COMPANY,INDIA CYCLE TRADING COMPANY,ISHAN  DXN HEALTH CARE</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>BABA PASHU AAHAR,BABA BRICKS FIELD,BABA BRICKS FIELD,BABA BRICKS FIELD,BABA BRICKS FIELD,BABA BRICKS FIELD,BABA GORAKHNATH IRON STORES,BABA JI MORDEN RICE MILL,BABA JI MORDEN RICE MILL,BABA MAHARAJ JI BRICK FIELD,BABA MAHARAJ JI BRICK FIELD,BABLU SINGH BUILDING  MATERIAL,BAIJNATH TRADERS,BAIJNATH TRADERS,BAJAJ BROTHERS,BAJRA SHAKTI IT BHATHA,BAJRA SHAKTI IT BHATHA,BAJRA SHAKTI IT BHATHA,BAJRANG BRICKS FIELD,BAJRANG BULLION TRADERS,BALA JI ENTERPRISES,BALAJI TRADERS,BALAJI TRADERS,BALVANT YADAV PLUMBRING WORKS,BALWANT SINGH BRICK FIELD,BALWANT SINGH BRICK FIELD,BALWANT SINGH BRICK FIELD,BALWANT SINGH BRICK FIELD,BALWANT SINGH BRICK FIELD,BHARAT PLASTIC,BHOLA HOSIERY,BISHESH TRADING COMPANY,BISWAS TRADERS,BISWAS TRADERS,BISWAS TRADERS,BOL BUM CONSTRUCTION,BOMBAY SURGICAL,BOMBAY SURGICAL,BOMBAY SURGICAL,BRIJMOHAN JAISWAL,BULLIAN TRADERS,BULLIAN TRADERS</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>HANUMANT BRICKS FIELD,HANUMANT BRICKS FIELD,HIMANSU TRADERS,HIMANSU TRADERS,HANUMANT ASSOCIATE,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI BRICKS FIELD,HARI OM TRADERS,HARI OM TRADERS,HARI OM TRADERS,HARIOM AUTOMOBILE,HARIOM AUTOMOBILE,HARISH CHANDRA JAISWAL,HARISH CHANDRA JAISWAL,HARISH CHANDRA JAISWAL,HARISH CHANDRA JAISWAL,HARSE  ENTERPRISES,HARSH  ENTERPRISES,HARSH  ENTERPRISES,HARSH ENTERPRISES,HARSHITA COAL ENTERPRISES,HEMANT BRICKS FIELD,HEMANT BRICKS FIELD,HEMANT BRICKS FIELD,HEMANT BRICKS FIELD,HEMANT BRICKS FIELD,HEMANT BRICKS FIELD,HIMALYA TRADERS,HIND CONSTRUCTIONS,HIND CONSTRUCTIONS,HINDUSTAN ALMIRAH,HOSIERY HOUSE,HINDUSTAN TRADERS,HINDUSTAN TRADERS,HINDUSTAN TRADERS,HINDUSTAN TRADERS,HINDUSTAN TRADERS</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>M.D. FAMILY SHOP,MAA SARYU ENTERPRISES AND OTHERS,MAHA LAXMI TEXTILES,MAHA LAXMI TEXTILES,M.B. NARAYAN,M.G.COPY MANUFACTURING UNIT,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,M.S TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA AMBEY TRADERS,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA ANNPURNA BRICKS FIELD,MAA BRICKS FIELD,MAA BRICKS FIELD,MAA BRICKS FIELD,MAA BRICKS FIELD,MAA CONSTRUCTION,MAA DURGA RICE MILL,MAA EENT UDYOG,MAA GAURI ASSOCIATES,MAA GAURI ASSOCIATES,MAA SAMAY BRICK FIELD,MAA SAMAY BRICK FIELD,MAA SAMAY BRICK FIELD,MAA SAMAY BRICK FIELD,MAA SAMAY BRICK FIELD,MAA SAMAY BRICK FIELD,MAA SAMAY BRICKS FIELD,MAA SAMAY BRICKS FIELD,MAA SHARDA AUTO MOBILE,MAA SHARDA AUTO MOBILE,MAA SHARDA PHARMA,MAA VAISHNO AUTOMOBILES,MAA VAISHNO AUTOMOBILES,MAA VAISHNO ENTERPRISES,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO GALLA BHANDAR,MAA VAISHNO MINI RICE MILL,MAA VAISHNO OIL AGENCY,MAA VAISHNO OIL AGENCY,MAA VAISHNO OIL AGENCY,MAA VAISHNO OIL AGENCY,MAA VAISHNO TRADERS,MAA VAISHNO TRADING COPMANY,MAA VAISHNO TRADRS,MAA VASHNO TRADERS,MAA VASHNO TRADERS,MADANESHWAR CHAND BKO.,MADANESHWAR CHAND BKO.,MADDHESIYA RICE MILL,MADHAV ENTERPRISES,MADHESHIYA RICE MILL,MADHESHIYA RICE MILL,MADHESHIYA RICE MILL,MADHESHIYA RICE MILL,MADHESIYA PACKING INDUSTRIES,MAHA LAXMI,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAHAVEER INT BHATTHA,MAK INTERPRISES,MAMATA AUTO MOBILS,MANISH TRADERS,MANISH TRADERS,MANISH TRADERS,MANOJ BRICKS FIELD,MANOJ BRICKS FIELD,MANOJ BRICKS FIELD,MANOJ BUILDING MATERIAL AND HARDWARE,MANOJ OPTICALS,MEERA DEVI,MEERA DEVI,MEERA DEVI,MEERA DEVI,MIRZA &amp; SONS,MIRZA &amp; SONS,MIRZA &amp; SONS,MISHRA INT UDYOG,MISHRA INT UDYOG,MISHRA INT UDYOG,MISHRA INT UDYOG,MISHRA INT UDYOG,MUNNA MOBILE SHOP,MURLI ENT BHATTHA UDYOG,MURLI ENT BHATTHA UDYOG,MURLI ENT BHATTHA UDYOG,MURLI ENT BHATTHA UDYOG,MURLI ENT BHATTHA UDYOG,MURLI ENTERPRISES,MAA AMBEY MARKETING AGENCY,MAA AMBEY MARKETING AGENCY,Mohd. Usman s/o Mohd. usuf</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>R. K. PLASTIC UDYOG,R. R. BROTHERS,R. R. BROTHERS,RADHA BRICKS UNIT,RAI AUTOMOBILE,RAI AUTOMOBILE,RAI AUTOMOBILE,RAI TRADERS,RAJ TRADERS,RAJESH ELECTRONCS AND MOBILE SHOP,RASMUNI AGENCIES,R.K.BRICKS FIELD,R.K.BRICKS FIELD,R.K.BRICKS FIELD,R.K.T.K.TRADERS,R.N. BRICKS FIELD,R.N. BRICKS FIELD,R.N. BRICKS FIELD,R.N.ENTERPRISES,R.P. BRIKS FILD,R.P. BRIKS FILD,R.P. BRIKS FILD,R.P. BRIKS FILD,R.P. BRIKS FILD,R.P. BRIKS FILD,R.S. ENTER PRISES,R.S.MARKETING &amp; COMPANY,R.S.MARKETING &amp; COMPANY,R.S.MARKETING &amp; COMPANY,RAHUL BRICKS FIELD,RAHUL BRICKS FIELD,RAHUL BRICKS FIELD,RAHUL BRICKS FIELD,RAHUL BRICKS FIELD,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAHUL EINT UDYOG,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAI BRICKS FIELD,RAJ AGENCIES,RAJ AGENCIES,RAJ TRADERS,RAJ TRADERS,RAJ TRADERS,RAJENDRA ENTERPRISES,RAJENDRA TRADERS,RAJESH GOEL JWELLERS,RAJESH JEWLLERS,RAJESH KUMAR SANJAY KUMAR,RAJESH KUMAR SANJAY KUMAR,RAJESHWAR KUMAR YADAV,RAJVEER CONSTRUCTION,RAM BELAS,RAM CHANDRA SURRAF,RAM CHANDRA SURRAF,RAM JI SUNIL KUMAR JEWELLERS,RAM KARAN YADAV GOVT CONTRACTOR AND SUPPLYER,RAM KUMAR SINGH,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM NAGEENA YADAV B.K.O,RAM PRASAD SUNIL KUMAR SARAF,RAMESH BRICKS FIELD,RAMESH BRICKS FIELD,RAMESH BRICKS FIELD,RAMESH BRICKS FIELD,RAMESH BRICKS FIELD,RAMUJAGIR TIWARI,RAVI PRATAP YADAV B.K.O.,RAVI PRATAP YADAV B.K.O.,RAVINDRA PRATAP SINGH B.K.O,RAVINDRA PRATAP SINGH B.K.O,RAVINDRA PRATAP SINGH B.K.O,RAVINDRA PRATAP SINGH B.K.O,RAVINDRA PRATAP SINGH B.K.O,RICHA H P GAS GRAMIN  VITARAK,RICHA H P GAS GRAMIN  VITARAK,RISHABH TRADERS,RISHI DRESSES,ROCKY MEDICAL STORES,ROCKY MEDICAL STORES,ROCKY MEDICAL STORES,ROSHNI ENTERPRISES,RAJEEV COMMUNICATION AND MOTORS,RAM CHANDER SWEET</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
     <t>LAL JI PRASAD,LAL JI PRASAD,LARI ALMIRA HOUSE,LARI TRUNK HOUSE,LARI TRUNK HOUSE,LAXMI TRADING COMPANY,LAXMI TRADING COMPANY,LOMA TRADERS,LOMA TRADERS,LUCKY ELECTRONICS,LUXMI ROADLINES,LUXMI TRADER'S,LUCKY ELECTRINIC</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>THAKUR PRASAD JWLLERS,THE  MAQBOOL STATIONERY STORES,THE  MAQBOOL STATIONERY STORES,TIRUPATI TRADERS,TRIPATHI TRADERS,TULASI ASSOCIATES,T.N.L.F. TRADERS</t>
   </si>
 </sst>
 </file>

</xml_diff>